<commit_message>
MANUAL CLEAN convo more minor edits [wiki examples dataset]
</commit_message>
<xml_diff>
--- a/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_clean/processed_step_3_manual_clean_convo.xlsx
+++ b/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_clean/processed_step_3_manual_clean_convo.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_label/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pongyizhen/Desktop/Github/SpeakSingapore/src/SpeakSingapore/data/wiki_examples_ERG/processed_step_3_manual_clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8E921D2-DA30-6F48-B228-744E131F4588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAEE790-A043-774F-9070-5ABEE0042379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -219,7 +219,81 @@
   </si>
   <si>
     <t xml:space="preserve">
-A: There is duty free sales on the plane. If you haven't bought it from the airport, you can buy here lah
+A: I screw up the physics test
+B: omg bro same... I didn't study the whole chapter on Electromagnetism
+A: Me too…I flung the whole paper, GG liao lor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: did you hear about the strike recently
+B: Yes postal service stopped. But in Singapore, if you strike you go to jail, don't know what they thinking
+A: Don't understand also, but they unhappy so like that lor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Hey, you are new here right?
+B: Yeap, first day in office
+A: Wah you look very handsome leh, like movie star
+B: haha thank you, I am flattered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: die lah
+B: how can immature females be allowed to choose their own life partner</t>
+  </si>
+  <si>
+    <t>Note</t>
+  </si>
+  <si>
+    <t>For some of the rows, it has been removed due inappropriate context varying from: 
+- incorrect use of Singlish particle
+- possibility of introducing various bias to LLM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">why changes to convo / not adopted </t>
+  </si>
+  <si>
+    <t>cleaned repetition</t>
+  </si>
+  <si>
+    <t>changed some context</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: Eh, who snitch on me lah
+B: Some bastard complain to teacher that I bring phone to school. Now it is confiscated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: I brought my phone to school today
+B: whattt, I am going to tell teacher
+A: Eh don’t backstab me leh
+</t>
+  </si>
+  <si>
+    <t>normalised sentence</t>
+  </si>
+  <si>
+    <t>incorrect use of lah</t>
+  </si>
+  <si>
+    <t>lah does not flow very well here</t>
+  </si>
+  <si>
+    <t>changed some context to retain leh and make context more appropriate</t>
+  </si>
+  <si>
+    <t>removed due to possible bias</t>
+  </si>
+  <si>
+    <t>removed due to inappropriate context</t>
+  </si>
+  <si>
+    <t>original sentence is not coherent (Singlish)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+A: There is duty free sales on the plane, you buy from here lah
 B: It's fine, no thank you
 A: The prices are better here
 B: Are you sure?
@@ -227,85 +301,11 @@
   </si>
   <si>
     <t xml:space="preserve">
-A: I screw up the physics test
-B: omg bro same... I didn't study the whole chapter on Electromagnetism
-A: Me too…I flung the whole paper, GG liao lor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
 A: Hey, what's up?
 B: My baby sneezed several times this morning.
 A: Oh no, is he sick?
-B: I don't know, but my wife insisted I should take him to the doctor [leh].
+B: I don't know, but my wife insisted I should take him to the doctor leh.
 A: I think he's just fine, tell your wife don't need to be so anxious</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A: did you hear about the strike recently
-B: Yes postal service stopped. But in Singapore, if you strike you go to jail, don't know what they thinking
-A: Don't understand also, but they unhappy so like that lor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A: Hey, you are new here right?
-B: Yeap, first day in office
-A: Wah you look very handsome leh, like movie star
-B: haha thank you, I am flattered</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A: die lah
-B: how can immature females be allowed to choose their own life partner</t>
-  </si>
-  <si>
-    <t>Note</t>
-  </si>
-  <si>
-    <t>For some of the rows, it has been removed due inappropriate context varying from: 
-- incorrect use of Singlish particle
-- possibility of introducing various bias to LLM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">why changes to convo / not adopted </t>
-  </si>
-  <si>
-    <t>cleaned repetition</t>
-  </si>
-  <si>
-    <t>changed some context</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A: Eh, who snitch on me lah
-B: Some bastard complain to teacher that I bring phone to school. Now it is confiscated</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-A: I brought my phone to school today
-B: whattt, I am going to tell teacher
-A: Eh don’t backstab me leh
-</t>
-  </si>
-  <si>
-    <t>normalised sentence</t>
-  </si>
-  <si>
-    <t>incorrect use of lah</t>
-  </si>
-  <si>
-    <t>lah does not flow very well here</t>
-  </si>
-  <si>
-    <t>changed some context to retain leh and make context more appropriate</t>
-  </si>
-  <si>
-    <t>removed due to possible bias</t>
-  </si>
-  <si>
-    <t>removed due to inappropriate context</t>
-  </si>
-  <si>
-    <t>original sentence is not coherent (Singlish)</t>
   </si>
 </sst>
 </file>
@@ -699,7 +699,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -707,7 +707,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -724,8 +724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -748,7 +748,7 @@
         <v>30</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -765,7 +765,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
@@ -782,7 +782,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.2">
@@ -793,13 +793,13 @@
         <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -810,13 +810,13 @@
         <v>19</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" t="b">
         <v>1</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="208" x14ac:dyDescent="0.2">
@@ -827,13 +827,13 @@
         <v>20</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D6" t="b">
         <v>1</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -844,13 +844,13 @@
         <v>21</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="176" x14ac:dyDescent="0.2">
@@ -867,7 +867,7 @@
         <v>0</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="96" x14ac:dyDescent="0.2">
@@ -884,7 +884,7 @@
         <v>0</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -895,13 +895,13 @@
         <v>24</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="112" x14ac:dyDescent="0.2">
@@ -912,13 +912,13 @@
         <v>25</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D11" t="b">
         <v>1</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="96" x14ac:dyDescent="0.2">
@@ -929,13 +929,13 @@
         <v>26</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" t="b">
         <v>1</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="160" x14ac:dyDescent="0.2">
@@ -946,13 +946,13 @@
         <v>27</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D13" t="b">
         <v>0</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -969,7 +969,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="128" x14ac:dyDescent="0.2">
@@ -986,7 +986,7 @@
         <v>0</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>